<commit_message>
Order was wrong, now should work
</commit_message>
<xml_diff>
--- a/_readme/programs-info.xlsx
+++ b/_readme/programs-info.xlsx
@@ -127,16 +127,16 @@
     <t xml:space="preserve">Processes the author and institution information, completing missing information</t>
   </si>
   <si>
-    <t xml:space="preserve">./programs/44_supplementary_authexp.R</t>
+    <t xml:space="preserve">./programs/44_supplementary_hindex.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-computes the h-index per author and year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./programs/45_supplementary_authexp.R</t>
   </si>
   <si>
     <t xml:space="preserve">This program primarily handles computing academic age of author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./programs/45_supplementary_hindex.R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Re-computes the h-index per author and year</t>
   </si>
   <si>
     <t xml:space="preserve">./programs/46_prepare_analysis.R</t>
@@ -412,7 +412,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -432,7 +432,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -440,7 +440,7 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -512,7 +512,7 @@
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -520,7 +520,7 @@
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -528,7 +528,7 @@
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -552,7 +552,7 @@
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -560,7 +560,7 @@
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -568,7 +568,7 @@
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -576,7 +576,7 @@
       <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -584,7 +584,7 @@
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -592,7 +592,7 @@
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -600,7 +600,7 @@
       <c r="A23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>44</v>
       </c>
     </row>
@@ -608,7 +608,7 @@
       <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>46</v>
       </c>
     </row>
@@ -616,7 +616,7 @@
       <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -624,7 +624,7 @@
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -632,7 +632,7 @@
       <c r="A27" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>52</v>
       </c>
     </row>
@@ -640,7 +640,7 @@
       <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>54</v>
       </c>
     </row>
@@ -648,7 +648,7 @@
       <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -656,7 +656,7 @@
       <c r="A30" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>58</v>
       </c>
     </row>
@@ -664,7 +664,7 @@
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>